<commit_message>
Evaluating a company using a ratio analysis
</commit_message>
<xml_diff>
--- a/_SaleSmart's+Financial+Ratios+Pack.xlsx
+++ b/_SaleSmart's+Financial+Ratios+Pack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365careers-my.sharepoint.com/personal/kristiana_365careers_onmicrosoft_com/Documents/CFA Level 1/4_Financial Reporting and Analysis/Reading 26 Financial Analysis Techniques/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/financial_ratio_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2819" documentId="114_{697FDD00-CAF3-4796-BCF2-12BA3BDDD244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{781B969C-CB2D-4CCD-B496-DEA752BE7708}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAADF2A-C3EC-D84D-95C7-9FA69ADBE4E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="950" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
+    <workbookView xWindow="5980" yWindow="560" windowWidth="23260" windowHeight="13180" tabRatio="950" xr2:uid="{40080B9E-9E5D-4D4F-BF78-D3F262E6937F}"/>
   </bookViews>
   <sheets>
     <sheet name="BS" sheetId="2" r:id="rId1"/>
@@ -34,9 +34,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2046,40 +2044,46 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2088,23 +2092,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2162,7 +2160,7 @@
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2484,36 +2482,36 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="C3" sqref="C3"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="3"/>
     <col min="4" max="4" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
       <c r="D6" s="63" t="s">
         <v>93</v>
       </c>
@@ -2521,7 +2519,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>87</v>
       </c>
@@ -2538,10 +2536,10 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="2:7" ht="12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
@@ -2550,7 +2548,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="2:7" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="6" t="s">
         <v>2</v>
       </c>
@@ -2559,7 +2557,7 @@
       <c r="E10" s="160"/>
       <c r="F10" s="160"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -2577,7 +2575,7 @@
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2594,7 +2592,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
@@ -2611,7 +2609,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B14" s="36" t="s">
         <v>7</v>
       </c>
@@ -2628,7 +2626,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" ht="13" x14ac:dyDescent="0.15">
       <c r="B15" s="6" t="s">
         <v>112</v>
       </c>
@@ -2647,14 +2645,14 @@
       </c>
       <c r="G15" s="35"/>
     </row>
-    <row r="16" spans="2:7" ht="12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
@@ -2662,7 +2660,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2680,7 +2678,7 @@
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
@@ -2699,7 +2697,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B20" s="4" t="s">
         <v>136</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>3045</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B21" s="36" t="s">
         <v>11</v>
       </c>
@@ -2733,7 +2731,7 @@
         <v>2998</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B22" s="6" t="s">
         <v>113</v>
       </c>
@@ -2751,7 +2749,7 @@
         <v>55590</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B23" s="28" t="s">
         <v>12</v>
       </c>
@@ -2769,13 +2767,13 @@
         <v>161553</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="4"/>
       <c r="C24" s="7"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B25" s="6" t="s">
         <v>13</v>
       </c>
@@ -2783,7 +2781,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="2:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B26" s="6" t="s">
         <v>109</v>
       </c>
@@ -2792,7 +2790,7 @@
       <c r="E26" s="64"/>
       <c r="F26" s="64"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B27" s="4" t="s">
         <v>185</v>
       </c>
@@ -2811,7 +2809,7 @@
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B28" s="4" t="s">
         <v>139</v>
       </c>
@@ -2827,7 +2825,7 @@
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B29" s="36" t="s">
         <v>14</v>
       </c>
@@ -2843,7 +2841,7 @@
       </c>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B30" s="6" t="s">
         <v>114</v>
       </c>
@@ -2861,7 +2859,7 @@
         <v>74537</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" ht="13" x14ac:dyDescent="0.15">
       <c r="B31" s="6" t="s">
         <v>15</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>24246</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B32" s="28" t="s">
         <v>16</v>
       </c>
@@ -2894,13 +2892,13 @@
         <v>98783</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="6"/>
       <c r="C33" s="260"/>
       <c r="D33" s="261"/>
       <c r="E33" s="261"/>
     </row>
-    <row r="34" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>17</v>
       </c>
@@ -2908,7 +2906,7 @@
       <c r="D34" s="262"/>
       <c r="E34" s="262"/>
     </row>
-    <row r="35" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
         <v>18</v>
       </c>
@@ -2917,7 +2915,7 @@
       <c r="E35" s="64"/>
       <c r="F35" s="64"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B36" s="4" t="s">
         <v>140</v>
       </c>
@@ -2934,7 +2932,7 @@
         <v>25781</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B37" s="4" t="s">
         <v>19</v>
       </c>
@@ -2951,7 +2949,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B38" s="36" t="s">
         <v>20</v>
       </c>
@@ -2968,7 +2966,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B39" s="6" t="s">
         <v>115</v>
       </c>
@@ -2986,14 +2984,14 @@
         <v>26827</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B40" s="6"/>
       <c r="C40" s="27"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
     </row>
-    <row r="41" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B41" s="6" t="s">
         <v>21</v>
       </c>
@@ -3002,7 +3000,7 @@
       <c r="E41" s="64"/>
       <c r="F41" s="64"/>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B42" s="4" t="s">
         <v>141</v>
       </c>
@@ -3019,7 +3017,7 @@
         <v>17970</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B43" s="4" t="s">
         <v>22</v>
       </c>
@@ -3036,7 +3034,7 @@
         <v>17802</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B44" s="4" t="s">
         <v>23</v>
       </c>
@@ -3051,7 +3049,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B45" s="6" t="s">
         <v>116</v>
       </c>
@@ -3069,7 +3067,7 @@
         <v>35943</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B46" s="32" t="s">
         <v>24</v>
       </c>
@@ -3087,7 +3085,7 @@
         <v>62770</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B47" s="28" t="s">
         <v>25</v>
       </c>
@@ -3105,7 +3103,7 @@
         <v>161553</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:7" x14ac:dyDescent="0.15">
       <c r="D49" s="10">
         <f>D47-D23</f>
         <v>0</v>
@@ -3144,26 +3142,26 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="19" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="1.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.83203125" style="3" customWidth="1"/>
     <col min="13" max="13" width="19" style="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.6640625" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="3"/>
+    <col min="15" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B3" s="242" t="s">
         <v>277</v>
       </c>
@@ -3183,41 +3181,41 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C5" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="273" t="s">
+      <c r="D5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="263" t="s">
         <v>99</v>
       </c>
       <c r="G5" s="40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C6" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="274"/>
+      <c r="D6" s="264"/>
       <c r="E6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="264"/>
       <c r="G6" s="41" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
       <c r="D7" s="76"/>
       <c r="F7" s="76"/>
     </row>
-    <row r="8" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B8" s="105" t="s">
         <v>164</v>
       </c>
@@ -3240,7 +3238,7 @@
         <v>1.6217682081396296</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B9" s="105" t="s">
         <v>165</v>
       </c>
@@ -3263,10 +3261,10 @@
         <v>1.6949262578505397</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B12" s="242" t="s">
         <v>278</v>
       </c>
@@ -3293,23 +3291,23 @@
       </c>
       <c r="J12" s="94"/>
     </row>
-    <row r="14" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C14" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="273" t="s">
+      <c r="D14" s="263" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="273" t="s">
+      <c r="F14" s="263" t="s">
         <v>99</v>
       </c>
       <c r="G14" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="273" t="s">
+      <c r="H14" s="263" t="s">
         <v>99</v>
       </c>
       <c r="I14" s="84" t="s">
@@ -3318,28 +3316,28 @@
       <c r="J14" s="75"/>
       <c r="K14" s="63"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C15" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="274"/>
+      <c r="D15" s="264"/>
       <c r="E15" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="274"/>
+      <c r="F15" s="264"/>
       <c r="G15" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="274"/>
+      <c r="H15" s="264"/>
       <c r="I15" s="85" t="s">
         <v>96</v>
       </c>
       <c r="J15" s="75"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.15">
       <c r="C16" s="56"/>
     </row>
-    <row r="17" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B17" s="105" t="s">
         <v>164</v>
       </c>
@@ -3370,7 +3368,7 @@
       </c>
       <c r="J17" s="95"/>
     </row>
-    <row r="18" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B18" s="105" t="s">
         <v>165</v>
       </c>
@@ -3401,7 +3399,7 @@
       </c>
       <c r="J18" s="95"/>
     </row>
-    <row r="21" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B21" s="242" t="s">
         <v>279</v>
       </c>
@@ -3439,7 +3437,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C23" s="88" t="s">
         <v>82</v>
       </c>
@@ -3474,7 +3472,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C24" s="91" t="s">
         <v>96</v>
       </c>
@@ -3499,7 +3497,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D25" s="26"/>
       <c r="E25" s="63"/>
       <c r="F25" s="26"/>
@@ -3510,7 +3508,7 @@
       <c r="K25" s="63"/>
       <c r="L25" s="26"/>
     </row>
-    <row r="26" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B26" s="105" t="s">
         <v>164</v>
       </c>
@@ -3554,7 +3552,7 @@
         <v>1.4252956528831253</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B27" s="105" t="s">
         <v>165</v>
       </c>
@@ -3600,16 +3598,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3625,19 +3623,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="205"/>
-    <col min="5" max="7" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="49.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="205"/>
+    <col min="5" max="7" width="8.83203125" style="3"/>
     <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:14" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D3" s="293" t="s">
         <v>223</v>
       </c>
@@ -3647,7 +3645,7 @@
       </c>
       <c r="G3" s="296"/>
     </row>
-    <row r="4" spans="2:14" s="144" customFormat="1" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" s="144" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B4" s="253" t="s">
         <v>180</v>
       </c>
@@ -3670,7 +3668,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B5" s="233" t="s">
         <v>211</v>
       </c>
@@ -3697,7 +3695,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B6" s="235" t="s">
         <v>212</v>
       </c>
@@ -3724,7 +3722,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B7" s="235" t="s">
         <v>213</v>
       </c>
@@ -3751,7 +3749,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B8" s="235" t="s">
         <v>210</v>
       </c>
@@ -3778,7 +3776,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="236" t="s">
         <v>214</v>
       </c>
@@ -3805,7 +3803,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B10" s="230" t="s">
         <v>224</v>
       </c>
@@ -3821,7 +3819,7 @@
         <v>2.2970209633392829</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.15">
       <c r="N11" s="3" t="s">
         <v>274</v>
       </c>
@@ -3845,18 +3843,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="13.77734375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="13.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:19" ht="12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.15">
       <c r="C3" s="297" t="s">
         <v>93</v>
       </c>
@@ -3868,7 +3866,7 @@
       <c r="G3" s="298"/>
       <c r="H3" s="299"/>
     </row>
-    <row r="4" spans="2:19" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B4" s="144"/>
       <c r="C4" s="257" t="s">
         <v>26</v>
@@ -3892,7 +3890,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B5" s="213" t="s">
         <v>249</v>
       </c>
@@ -3921,7 +3919,7 @@
         <v>2.218259949132273E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B6" s="218" t="s">
         <v>225</v>
       </c>
@@ -3950,7 +3948,7 @@
         <v>2.3949579831932771E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B7" s="218" t="s">
         <v>250</v>
       </c>
@@ -3979,7 +3977,7 @@
         <v>5.4049935992958043E-3</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B8" s="218" t="s">
         <v>252</v>
       </c>
@@ -4008,7 +4006,7 @@
         <v>2.7451200972465006E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B9" s="219" t="s">
         <v>251</v>
       </c>
@@ -4038,7 +4036,7 @@
       </c>
       <c r="S9" s="220"/>
     </row>
-    <row r="10" spans="2:19" s="144" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" s="144" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="221" t="s">
         <v>228</v>
       </c>
@@ -4071,14 +4069,14 @@
         <v>1.3661152479096689E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.15">
       <c r="C11" s="140"/>
       <c r="D11" s="140"/>
       <c r="E11" s="19"/>
       <c r="F11" s="141"/>
       <c r="G11" s="141"/>
     </row>
-    <row r="13" spans="2:19" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.15">
       <c r="C13" s="297" t="s">
         <v>93</v>
       </c>
@@ -4090,7 +4088,7 @@
       <c r="G13" s="298"/>
       <c r="H13" s="299"/>
     </row>
-    <row r="14" spans="2:19" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.15">
       <c r="C14" s="257" t="s">
         <v>26</v>
       </c>
@@ -4110,7 +4108,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B15" s="213" t="s">
         <v>229</v>
       </c>
@@ -4135,7 +4133,7 @@
         <v>0.18011265317653707</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B16" s="218" t="s">
         <v>230</v>
       </c>
@@ -4160,7 +4158,7 @@
         <v>0.24039408866995074</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B17" s="218" t="s">
         <v>253</v>
       </c>
@@ -4185,7 +4183,7 @@
         <v>0.43253530240170518</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B18" s="221" t="s">
         <v>228</v>
       </c>
@@ -4241,35 +4239,35 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="6" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="25" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="25"/>
     </row>
-    <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="25"/>
       <c r="D7" s="63" t="s">
         <v>93</v>
@@ -4278,7 +4276,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="12.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>87</v>
       </c>
@@ -4292,13 +4290,13 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="5"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
@@ -4306,7 +4304,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>27</v>
       </c>
@@ -4320,7 +4318,7 @@
         <v>172829</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
@@ -4334,7 +4332,7 @@
         <v>7312</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>110</v>
       </c>
@@ -4348,13 +4346,13 @@
         <v>180141</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B15" s="4" t="s">
         <v>138</v>
       </c>
@@ -4367,14 +4365,14 @@
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="28" t="s">
         <v>39</v>
       </c>
@@ -4388,13 +4386,13 @@
         <v>41525.160000000003</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B18" s="6"/>
       <c r="C18" s="2"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
@@ -4406,7 +4404,7 @@
         <v>-4906.32</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B20" s="4" t="s">
         <v>68</v>
       </c>
@@ -4418,7 +4416,7 @@
         <v>-15989.84</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B21" s="4" t="s">
         <v>29</v>
       </c>
@@ -4430,7 +4428,7 @@
         <v>-2032</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B22" s="28" t="s">
         <v>111</v>
       </c>
@@ -4444,13 +4442,13 @@
         <v>-22928.16</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B23" s="4"/>
       <c r="C23" s="2"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B24" s="28" t="s">
         <v>166</v>
       </c>
@@ -4464,13 +4462,13 @@
         <v>18597.000000000004</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B26" s="4" t="s">
         <v>137</v>
       </c>
@@ -4484,13 +4482,13 @@
         <v>-2992</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="4"/>
       <c r="C27" s="7"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B28" s="28" t="s">
         <v>167</v>
       </c>
@@ -4504,13 +4502,13 @@
         <v>15605.000000000004</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B29" s="16"/>
       <c r="C29" s="17"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" ht="13" x14ac:dyDescent="0.15">
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
@@ -4525,13 +4523,13 @@
       </c>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B31" s="16"/>
       <c r="C31" s="17"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
     </row>
-    <row r="32" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B32" s="28" t="s">
         <v>97</v>
       </c>
@@ -4545,13 +4543,13 @@
         <v>13962.000000000004</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="18"/>
       <c r="C33" s="17"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="2:6" ht="12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
         <v>31</v>
       </c>
@@ -4559,7 +4557,7 @@
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
@@ -4571,7 +4569,7 @@
         <v>10006</v>
       </c>
     </row>
-    <row r="36" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="B36" s="36" t="s">
         <v>15</v>
       </c>
@@ -4584,7 +4582,7 @@
       </c>
       <c r="F36" s="35"/>
     </row>
-    <row r="37" spans="2:6" ht="12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" hidden="1" x14ac:dyDescent="0.15">
       <c r="B37" s="4"/>
       <c r="C37" s="2"/>
       <c r="D37" s="13">
@@ -4597,7 +4595,7 @@
       </c>
       <c r="F37" s="35"/>
     </row>
-    <row r="38" spans="2:6" ht="12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="B38" s="6" t="s">
         <v>33</v>
       </c>
@@ -4605,7 +4603,7 @@
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
     </row>
-    <row r="39" spans="2:6" ht="22.8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" ht="26" hidden="1" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
@@ -4613,7 +4611,7 @@
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
     </row>
-    <row r="40" spans="2:6" ht="22.8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" ht="26" hidden="1" x14ac:dyDescent="0.15">
       <c r="B40" s="4" t="s">
         <v>35</v>
       </c>
@@ -4625,7 +4623,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="24.6" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B41" s="28" t="s">
         <v>36</v>
       </c>
@@ -4639,13 +4637,13 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" hidden="1" x14ac:dyDescent="0.15">
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
     </row>
-    <row r="43" spans="2:6" ht="24.6" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="27" hidden="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B43" s="28" t="s">
         <v>37</v>
       </c>
@@ -4659,13 +4657,13 @@
         <v>14999</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" hidden="1" x14ac:dyDescent="0.15">
       <c r="B44" s="18"/>
       <c r="C44" s="17"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
     </row>
-    <row r="45" spans="2:6" ht="24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" ht="26" hidden="1" x14ac:dyDescent="0.15">
       <c r="B45" s="6" t="s">
         <v>38</v>
       </c>
@@ -4673,7 +4671,7 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="B46" s="4" t="s">
         <v>32</v>
       </c>
@@ -4686,7 +4684,7 @@
       </c>
       <c r="F46" s="35"/>
     </row>
-    <row r="47" spans="2:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" ht="13" hidden="1" x14ac:dyDescent="0.15">
       <c r="B47" s="36" t="s">
         <v>15</v>
       </c>
@@ -4699,7 +4697,7 @@
       </c>
       <c r="F47" s="35"/>
     </row>
-    <row r="48" spans="2:6" ht="12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" hidden="1" x14ac:dyDescent="0.15">
       <c r="B48" s="4"/>
       <c r="C48" s="7"/>
       <c r="D48" s="13">
@@ -4712,14 +4710,14 @@
       </c>
       <c r="F48" s="35"/>
     </row>
-    <row r="49" spans="2:6" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
       <c r="C49" s="112"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="35"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B50" s="114" t="s">
         <v>186</v>
       </c>
@@ -4731,7 +4729,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B51" s="118" t="s">
         <v>198</v>
       </c>
@@ -4743,7 +4741,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B52" s="118" t="s">
         <v>203</v>
       </c>
@@ -4757,7 +4755,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B53" s="118" t="s">
         <v>190</v>
       </c>
@@ -4769,7 +4767,7 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B54" s="115" t="s">
         <v>192</v>
       </c>
@@ -4783,7 +4781,7 @@
         <v>21500</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B55" s="243" t="s">
         <v>81</v>
       </c>
@@ -4808,27 +4806,29 @@
   </sheetPr>
   <dimension ref="B3:O49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.21875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="37.109375" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="37.1640625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" s="70" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="269" t="s">
         <v>105</v>
       </c>
@@ -4851,8 +4851,8 @@
       </c>
       <c r="O3" s="158"/>
     </row>
-    <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="267" t="s">
+    <row r="5" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="265" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -4862,7 +4862,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="53">
@@ -4873,19 +4873,19 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J5" s="273" t="s">
+      <c r="J5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K5" s="53">
         <f>I5/I6</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="267" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="268"/>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B6" s="266"/>
       <c r="C6" s="41" t="s">
         <v>43</v>
       </c>
@@ -4893,26 +4893,26 @@
         <f>AVERAGE(BS!D19:E19)</f>
         <v>25432</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="264"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>AVERAGE(BS!E19:F19)</f>
         <v>25366</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="264"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="264"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="268"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="10"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I8" s="10"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="2:15" ht="12" x14ac:dyDescent="0.25">
-      <c r="B9" s="267" t="s">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B9" s="265" t="s">
         <v>119</v>
       </c>
       <c r="C9" s="40">
@@ -4921,7 +4921,7 @@
       <c r="E9" s="59">
         <v>365</v>
       </c>
-      <c r="F9" s="273" t="s">
+      <c r="F9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="53">
@@ -4931,19 +4931,19 @@
       <c r="I9" s="59">
         <v>365</v>
       </c>
-      <c r="J9" s="273" t="s">
+      <c r="J9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="53">
         <f>I9/I10</f>
         <v>51.396350636445895</v>
       </c>
-      <c r="M9" s="263" t="s">
+      <c r="M9" s="267" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="268"/>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B10" s="266"/>
       <c r="C10" s="41" t="s">
         <v>45</v>
       </c>
@@ -4951,26 +4951,26 @@
         <f>G5</f>
         <v>7.8186929852154767</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="264"/>
       <c r="G10" s="46"/>
       <c r="I10" s="60">
         <f>K5</f>
         <v>7.1016715288181027</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="264"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="264"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M10" s="268"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="10"/>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I12" s="10"/>
       <c r="J12" s="21"/>
     </row>
-    <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="267" t="s">
+    <row r="13" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="265" t="s">
         <v>118</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -4980,7 +4980,7 @@
         <f>-'P&amp;L'!D15</f>
         <v>150291.84</v>
       </c>
-      <c r="F13" s="273" t="s">
+      <c r="F13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="44">
@@ -4991,19 +4991,19 @@
         <f>-'P&amp;L'!E15</f>
         <v>138615.84</v>
       </c>
-      <c r="J13" s="273" t="s">
+      <c r="J13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="267" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="268"/>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B14" s="266"/>
       <c r="C14" s="41" t="s">
         <v>47</v>
       </c>
@@ -5011,26 +5011,26 @@
         <f>AVERAGE(BS!D18:E18)</f>
         <v>24563.5</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="264"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>AVERAGE(BS!E18:F18)</f>
         <v>23595</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="264"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="264"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M14" s="268"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I15" s="10"/>
       <c r="J15" s="21"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I16" s="10"/>
       <c r="J16" s="21"/>
     </row>
-    <row r="17" spans="2:14" ht="12" x14ac:dyDescent="0.25">
-      <c r="B17" s="267" t="s">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B17" s="265" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="40">
@@ -5039,7 +5039,7 @@
       <c r="E17" s="59">
         <v>365</v>
       </c>
-      <c r="F17" s="273" t="s">
+      <c r="F17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="53">
@@ -5049,19 +5049,19 @@
       <c r="I17" s="59">
         <v>365</v>
       </c>
-      <c r="J17" s="273" t="s">
+      <c r="J17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="53">
         <f>I17/I18</f>
         <v>62.129804212851859</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="267" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="268"/>
+    <row r="18" spans="2:14" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="266"/>
       <c r="C18" s="41" t="s">
         <v>49</v>
       </c>
@@ -5069,26 +5069,26 @@
         <f>G13</f>
         <v>6.1185026563804019</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="264"/>
       <c r="G18" s="46"/>
       <c r="I18" s="57">
         <f>K13</f>
         <v>5.8747972027972031</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="264"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="264"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M18" s="268"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I19" s="10"/>
       <c r="J19" s="21"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I20" s="10"/>
       <c r="J20" s="21"/>
     </row>
-    <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="267" t="s">
+    <row r="21" spans="2:14" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="265" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -5098,7 +5098,7 @@
         <f>BS!D18-BS!E18+(-'P&amp;L'!D15)</f>
         <v>151902.84</v>
       </c>
-      <c r="F21" s="273" t="s">
+      <c r="F21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="44">
@@ -5109,22 +5109,22 @@
         <f>BS!E18-BS!F18+(-'P&amp;L'!E15)</f>
         <v>138941.84</v>
       </c>
-      <c r="J21" s="273" t="s">
+      <c r="J21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K21" s="44">
         <f>I21/I22</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="267" t="s">
         <v>244</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="268"/>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B22" s="266"/>
       <c r="C22" s="41" t="s">
         <v>52</v>
       </c>
@@ -5132,26 +5132,26 @@
         <f>AVERAGE(BS!D43:E43)</f>
         <v>18397.5</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="264"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E43:F43)</f>
         <v>17949</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="264"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="264"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M22" s="268"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I23" s="10"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I24" s="10"/>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="2:14" ht="12" x14ac:dyDescent="0.25">
-      <c r="B25" s="267" t="s">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B25" s="265" t="s">
         <v>122</v>
       </c>
       <c r="C25" s="40">
@@ -5160,7 +5160,7 @@
       <c r="E25" s="59">
         <v>365</v>
       </c>
-      <c r="F25" s="273" t="s">
+      <c r="F25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G25" s="53">
@@ -5170,19 +5170,19 @@
       <c r="I25" s="59">
         <v>365</v>
       </c>
-      <c r="J25" s="273" t="s">
+      <c r="J25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K25" s="53">
         <f>I25/I26</f>
         <v>47.151995396059242</v>
       </c>
-      <c r="M25" s="265" t="s">
+      <c r="M25" s="273" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="268"/>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B26" s="266"/>
       <c r="C26" s="41" t="s">
         <v>53</v>
       </c>
@@ -5190,26 +5190,26 @@
         <f>G21</f>
         <v>8.2567109661638813</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="264"/>
       <c r="G26" s="46"/>
       <c r="I26" s="57">
         <f>K21</f>
         <v>7.7409237283414116</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="264"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="266"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M26" s="274"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I27" s="10"/>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I28" s="10"/>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="267" t="s">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B29" s="265" t="s">
         <v>124</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -5219,7 +5219,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F29" s="273" t="s">
+      <c r="F29" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G29" s="44">
@@ -5230,19 +5230,19 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J29" s="273" t="s">
+      <c r="J29" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K29" s="44">
         <f>I29/I30</f>
         <v>1.72279045747321</v>
       </c>
-      <c r="M29" s="263" t="s">
+      <c r="M29" s="267" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="268"/>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B30" s="266"/>
       <c r="C30" s="41" t="s">
         <v>56</v>
       </c>
@@ -5250,26 +5250,26 @@
         <f>AVERAGE(BS!D11:E11)</f>
         <v>106074.5</v>
       </c>
-      <c r="F30" s="274"/>
+      <c r="F30" s="264"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E11:F11)</f>
         <v>104563.5</v>
       </c>
-      <c r="J30" s="274"/>
+      <c r="J30" s="264"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="264"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M30" s="268"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I31" s="10"/>
       <c r="J31" s="21"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.15">
       <c r="I32" s="10"/>
       <c r="J32" s="21"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B33" s="267" t="s">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B33" s="265" t="s">
         <v>125</v>
       </c>
       <c r="C33" s="40" t="s">
@@ -5279,7 +5279,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F33" s="273" t="s">
+      <c r="F33" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G33" s="44">
@@ -5290,19 +5290,19 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J33" s="273" t="s">
+      <c r="J33" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K33" s="44">
         <f>I33/I34</f>
         <v>7.4487677803506447</v>
       </c>
-      <c r="M33" s="263" t="s">
+      <c r="M33" s="267" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="268"/>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B34" s="266"/>
       <c r="C34" s="41" t="s">
         <v>57</v>
       </c>
@@ -5310,17 +5310,17 @@
         <f>AVERAGE(BS!D22:E22)-AVERAGE(BS!D45:E45)</f>
         <v>34063</v>
       </c>
-      <c r="F34" s="274"/>
+      <c r="F34" s="264"/>
       <c r="G34" s="46"/>
       <c r="I34" s="45">
         <f>AVERAGE(BS!E22:F22)-AVERAGE(BS!E45:F45)</f>
         <v>24184</v>
       </c>
-      <c r="J34" s="274"/>
+      <c r="J34" s="264"/>
       <c r="K34" s="46"/>
-      <c r="M34" s="264"/>
-    </row>
-    <row r="35" spans="2:13" ht="12" x14ac:dyDescent="0.2">
+      <c r="M34" s="268"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B35" s="61"/>
       <c r="C35" s="56"/>
       <c r="E35" s="62"/>
@@ -5330,12 +5330,12 @@
       <c r="J35" s="56"/>
       <c r="K35" s="35"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I36" s="10"/>
       <c r="J36" s="21"/>
     </row>
-    <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="267" t="s">
+    <row r="37" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="265" t="s">
         <v>126</v>
       </c>
       <c r="C37" s="40" t="s">
@@ -5345,7 +5345,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F37" s="273" t="s">
+      <c r="F37" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G37" s="44">
@@ -5356,19 +5356,19 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J37" s="273" t="s">
+      <c r="J37" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K37" s="44">
         <f>I37/I38</f>
         <v>1.0923495329312995</v>
       </c>
-      <c r="M37" s="263" t="s">
+      <c r="M37" s="267" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="268"/>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B38" s="266"/>
       <c r="C38" s="41" t="s">
         <v>55</v>
       </c>
@@ -5376,25 +5376,25 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F38" s="274"/>
+      <c r="F38" s="264"/>
       <c r="G38" s="46"/>
       <c r="I38" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J38" s="274"/>
+      <c r="J38" s="264"/>
       <c r="K38" s="46"/>
-      <c r="M38" s="264"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M38" s="268"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I39" s="10"/>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.15">
       <c r="I40" s="10"/>
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="2:13" ht="12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B41" s="47" t="s">
         <v>127</v>
       </c>
@@ -5424,11 +5424,11 @@
         <f>I41+I43-I45</f>
         <v>66.374159453238519</v>
       </c>
-      <c r="M41" s="263" t="s">
+      <c r="M41" s="267" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B42" s="49"/>
       <c r="C42" s="50"/>
       <c r="D42" s="3"/>
@@ -5444,7 +5444,7 @@
       <c r="K42" s="50"/>
       <c r="M42" s="272"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B43" s="49"/>
       <c r="C43" s="50" t="s">
         <v>103</v>
@@ -5464,7 +5464,7 @@
       <c r="K43" s="50"/>
       <c r="M43" s="272"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B44" s="49"/>
       <c r="C44" s="50"/>
       <c r="E44" s="54" t="s">
@@ -5479,7 +5479,7 @@
       <c r="K44" s="50"/>
       <c r="M44" s="272"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B45" s="51"/>
       <c r="C45" s="46" t="s">
         <v>121</v>
@@ -5496,14 +5496,14 @@
       </c>
       <c r="J45" s="20"/>
       <c r="K45" s="46"/>
-      <c r="M45" s="264"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M45" s="268"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.15">
       <c r="E46" s="21"/>
       <c r="K46" s="21"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="267" t="s">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B48" s="265" t="s">
         <v>128</v>
       </c>
       <c r="C48" s="40" t="s">
@@ -5513,7 +5513,7 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F48" s="273" t="s">
+      <c r="F48" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G48" s="44">
@@ -5524,19 +5524,19 @@
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J48" s="273" t="s">
+      <c r="J48" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K48" s="44">
         <f>I48/I49</f>
         <v>1.6949262578505397</v>
       </c>
-      <c r="M48" s="263" t="s">
+      <c r="M48" s="267" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B49" s="268"/>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B49" s="266"/>
       <c r="C49" s="41" t="s">
         <v>76</v>
       </c>
@@ -5544,18 +5544,46 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F49" s="274"/>
+      <c r="F49" s="264"/>
       <c r="G49" s="46"/>
       <c r="I49" s="45">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J49" s="274"/>
+      <c r="J49" s="264"/>
       <c r="K49" s="46"/>
-      <c r="M49" s="264"/>
+      <c r="M49" s="268"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="M41:M45"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="B37:B38"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="F37:F38"/>
@@ -5572,34 +5600,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="M41:M45"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M13:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5617,25 +5617,25 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="3" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="6" style="3" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="41.109375" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="41.1640625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" s="70" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="269" t="s">
         <v>105</v>
       </c>
@@ -5657,8 +5657,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="267" t="s">
+    <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="265" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5669,7 +5669,7 @@
         <f>BS!D22</f>
         <v>70907</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="44">
@@ -5680,19 +5680,19 @@
         <f>BS!E22</f>
         <v>61001</v>
       </c>
-      <c r="J5" s="273" t="s">
+      <c r="J5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K5" s="44">
         <f>I5/I6</f>
         <v>1.8897459727385377</v>
       </c>
-      <c r="M5" s="265" t="s">
+      <c r="M5" s="273" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="268"/>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B6" s="266"/>
       <c r="C6" s="41" t="s">
         <v>60</v>
       </c>
@@ -5701,18 +5701,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="264"/>
       <c r="G6" s="46"/>
       <c r="I6" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="264"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="266"/>
-    </row>
-    <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="267" t="s">
+      <c r="M6" s="274"/>
+    </row>
+    <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="265" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -5723,7 +5723,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F9" s="273" t="s">
+      <c r="F9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="44">
@@ -5734,19 +5734,19 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J9" s="273" t="s">
+      <c r="J9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="44">
         <f>I9/I10</f>
         <v>1.1537484510532838</v>
       </c>
-      <c r="M9" s="265" t="s">
+      <c r="M9" s="273" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="268"/>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B10" s="266"/>
       <c r="C10" s="41" t="s">
         <v>60</v>
       </c>
@@ -5755,18 +5755,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="264"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="264"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="266"/>
-    </row>
-    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="267" t="s">
+      <c r="M10" s="274"/>
+    </row>
+    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="265" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -5777,7 +5777,7 @@
         <f>SUM(BS!D20:D21)</f>
         <v>19291</v>
       </c>
-      <c r="F13" s="273" t="s">
+      <c r="F13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="44">
@@ -5788,19 +5788,19 @@
         <f>SUM(BS!E20:E21)</f>
         <v>12626</v>
       </c>
-      <c r="J13" s="273" t="s">
+      <c r="J13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K13" s="44">
         <f>I13/I14</f>
         <v>0.39114002478314747</v>
       </c>
-      <c r="M13" s="265" t="s">
+      <c r="M13" s="273" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="268"/>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B14" s="266"/>
       <c r="C14" s="41" t="s">
         <v>60</v>
       </c>
@@ -5809,18 +5809,18 @@
         <f>BS!D45</f>
         <v>31502</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="264"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>BS!E45</f>
         <v>32280</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="264"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="266"/>
-    </row>
-    <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="267" t="s">
+      <c r="M14" s="274"/>
+    </row>
+    <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="265" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -5831,7 +5831,7 @@
         <f>SUM(BS!D19:D21)</f>
         <v>45538</v>
       </c>
-      <c r="F17" s="273" t="s">
+      <c r="F17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="44">
@@ -5842,19 +5842,19 @@
         <f>SUM(BS!E19:E21)</f>
         <v>37243</v>
       </c>
-      <c r="J17" s="273" t="s">
+      <c r="J17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="44">
         <f>I17/I18</f>
         <v>84.148560144604573</v>
       </c>
-      <c r="M17" s="265" t="s">
+      <c r="M17" s="273" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="268"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B18" s="266"/>
       <c r="C18" s="41" t="s">
         <v>66</v>
       </c>
@@ -5863,27 +5863,18 @@
         <f>-('P&amp;L'!D15+'P&amp;L'!D19+'P&amp;L'!D20+'P&amp;L'!D21)/365</f>
         <v>482.99726027397259</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="264"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>-('P&amp;L'!E15+'P&amp;L'!E19+'P&amp;L'!E20+'P&amp;L'!E21)/365</f>
         <v>442.58630136986301</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="264"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="266"/>
+      <c r="M18" s="274"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="M5:M6"/>
@@ -5894,6 +5885,15 @@
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5909,25 +5909,25 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" style="19" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.77734375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="3" customWidth="1"/>
     <col min="13" max="13" width="24.33203125" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" s="70" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" s="70" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="269" t="s">
         <v>105</v>
       </c>
@@ -5949,8 +5949,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="267" t="s">
+    <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="265" t="s">
         <v>69</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -5961,7 +5961,7 @@
         <f>BS!D42+BS!D36</f>
         <v>29474</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="66">
@@ -5972,19 +5972,19 @@
         <f>BS!E42+BS!E36</f>
         <v>35016</v>
       </c>
-      <c r="J5" s="273" t="s">
+      <c r="J5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K5" s="66">
         <f>I5/I6</f>
         <v>0.30774639222372607</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="267" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="268"/>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B6" s="266"/>
       <c r="C6" s="41" t="s">
         <v>72</v>
       </c>
@@ -5993,17 +5993,17 @@
         <f>BS!D32</f>
         <v>131438</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="264"/>
       <c r="G6" s="67"/>
       <c r="I6" s="45">
         <f>BS!E32</f>
         <v>113782</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="264"/>
       <c r="K6" s="67"/>
-      <c r="M6" s="264"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M6" s="268"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
       <c r="E7" s="10"/>
       <c r="F7" s="21"/>
@@ -6011,7 +6011,7 @@
       <c r="J7" s="21"/>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D8" s="21"/>
       <c r="E8" s="10"/>
       <c r="F8" s="21"/>
@@ -6019,8 +6019,8 @@
       <c r="J8" s="21"/>
       <c r="K8" s="19"/>
     </row>
-    <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="267" t="s">
+    <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="265" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6031,7 +6031,7 @@
         <f>BS!D36+BS!D42</f>
         <v>29474</v>
       </c>
-      <c r="F9" s="273" t="s">
+      <c r="F9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="66">
@@ -6042,19 +6042,19 @@
         <f>BS!E36+BS!E42</f>
         <v>35016</v>
       </c>
-      <c r="J9" s="273" t="s">
+      <c r="J9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="66">
         <f>I9/I10</f>
         <v>0.23532574362558636</v>
       </c>
-      <c r="M9" s="263" t="s">
+      <c r="M9" s="267" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="268"/>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B10" s="266"/>
       <c r="C10" s="41" t="s">
         <v>73</v>
       </c>
@@ -6063,24 +6063,24 @@
         <f>BS!D36+BS!D42+BS!D32</f>
         <v>160912</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="264"/>
       <c r="G10" s="67"/>
       <c r="I10" s="65">
         <f>BS!E36+BS!E42+BS!E32</f>
         <v>148798</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="264"/>
       <c r="K10" s="67"/>
-      <c r="M10" s="264"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M10" s="268"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K11" s="19"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="267" t="s">
+    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="265" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6091,7 +6091,7 @@
         <f>BS!D36+BS!D42</f>
         <v>29474</v>
       </c>
-      <c r="F13" s="273" t="s">
+      <c r="F13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="66">
@@ -6102,19 +6102,19 @@
         <f>BS!E36+BS!E42</f>
         <v>35016</v>
       </c>
-      <c r="J13" s="273" t="s">
+      <c r="J13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K13" s="66">
         <f>I13/I14</f>
         <v>0.20809413442681404</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="267" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="268"/>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B14" s="266"/>
       <c r="C14" s="41" t="s">
         <v>74</v>
       </c>
@@ -6123,24 +6123,24 @@
         <f>BS!D23</f>
         <v>181241</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="264"/>
       <c r="G14" s="67"/>
       <c r="I14" s="65">
         <f>BS!E23</f>
         <v>168270</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="264"/>
       <c r="K14" s="67"/>
-      <c r="M14" s="264"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M14" s="268"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K15" s="19"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K16" s="19"/>
     </row>
-    <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="267" t="s">
+    <row r="17" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="265" t="s">
         <v>280</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6151,7 +6151,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F17" s="273" t="s">
+      <c r="F17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="71">
@@ -6162,19 +6162,19 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J17" s="273" t="s">
+      <c r="J17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="71">
         <f>I17/I18</f>
         <v>6.2155748663101615</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="267" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="268"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B18" s="266"/>
       <c r="C18" s="41" t="s">
         <v>78</v>
       </c>
@@ -6183,24 +6183,24 @@
         <f>-'P&amp;L'!D26</f>
         <v>2725</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="264"/>
       <c r="G18" s="67"/>
       <c r="I18" s="65">
         <f>-'P&amp;L'!E26</f>
         <v>2992</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="264"/>
       <c r="K18" s="67"/>
-      <c r="M18" s="264"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M18" s="268"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K19" s="19"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K20" s="19"/>
     </row>
-    <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="267" t="s">
+    <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="265" t="s">
         <v>281</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6211,7 +6211,7 @@
         <f>'P&amp;L'!D24-'P&amp;L'!D55</f>
         <v>24832.000000000004</v>
       </c>
-      <c r="F21" s="273" t="s">
+      <c r="F21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="71">
@@ -6222,19 +6222,19 @@
         <f>'P&amp;L'!E24-'P&amp;L'!E55</f>
         <v>21072.000000000004</v>
       </c>
-      <c r="J21" s="273" t="s">
+      <c r="J21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K21" s="71">
         <f>I21/I22</f>
         <v>3.8543991220047564</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="267" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="268"/>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B22" s="266"/>
       <c r="C22" s="41" t="s">
         <v>80</v>
       </c>
@@ -6243,21 +6243,21 @@
         <f>-'P&amp;L'!D26-'P&amp;L'!D55</f>
         <v>5006</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="264"/>
       <c r="G22" s="67"/>
       <c r="I22" s="65">
         <f>-'P&amp;L'!E26-'P&amp;L'!E55</f>
         <v>5467</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="264"/>
       <c r="K22" s="67"/>
-      <c r="M22" s="264"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M22" s="268"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.15">
       <c r="K24" s="19"/>
     </row>
-    <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="267" t="s">
+    <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="265" t="s">
         <v>282</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6268,7 +6268,7 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F25" s="273" t="s">
+      <c r="F25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G25" s="71">
@@ -6279,19 +6279,19 @@
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J25" s="273" t="s">
+      <c r="J25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K25" s="71">
         <f>I25/I26</f>
         <v>1.5516336179521557</v>
       </c>
-      <c r="M25" s="263" t="s">
+      <c r="M25" s="267" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="268"/>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B26" s="266"/>
       <c r="C26" s="41" t="s">
         <v>76</v>
       </c>
@@ -6300,28 +6300,25 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="264"/>
       <c r="G26" s="67"/>
       <c r="I26" s="65">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="264"/>
       <c r="K26" s="67"/>
-      <c r="M26" s="264"/>
+      <c r="M26" s="268"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B25:B26"/>
@@ -6332,13 +6329,16 @@
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6354,25 +6354,25 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="7" style="3" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="33.21875" style="76" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="12" max="12" width="2.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="33.1640625" style="76" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" s="70" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="269" t="s">
         <v>105</v>
       </c>
@@ -6394,15 +6394,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D4" s="21"/>
       <c r="E4" s="10"/>
       <c r="F4" s="21"/>
       <c r="I4" s="10"/>
       <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="267" t="s">
+    <row r="5" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="265" t="s">
         <v>175</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6413,7 +6413,7 @@
         <f>'P&amp;L'!D17</f>
         <v>48553.16</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="72">
@@ -6424,19 +6424,19 @@
         <f>'P&amp;L'!E17</f>
         <v>41525.160000000003</v>
       </c>
-      <c r="J5" s="273" t="s">
+      <c r="J5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K5" s="72">
         <f>I5/I6</f>
         <v>0.23051476343530902</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="267" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="268"/>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B6" s="266"/>
       <c r="C6" s="41" t="s">
         <v>54</v>
       </c>
@@ -6445,32 +6445,32 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="264"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="264"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="264"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M6" s="268"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D7" s="21"/>
       <c r="E7" s="10"/>
       <c r="F7" s="21"/>
       <c r="I7" s="10"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D8" s="21"/>
       <c r="E8" s="10"/>
       <c r="F8" s="21"/>
       <c r="I8" s="10"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="267" t="s">
+    <row r="9" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="265" t="s">
         <v>176</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -6481,7 +6481,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F9" s="273" t="s">
+      <c r="F9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="72">
@@ -6492,19 +6492,19 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J9" s="273" t="s">
+      <c r="J9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="72">
         <f>I9/I10</f>
         <v>0.1032357986244109</v>
       </c>
-      <c r="M9" s="263" t="s">
+      <c r="M9" s="267" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="268"/>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B10" s="266"/>
       <c r="C10" s="41" t="s">
         <v>54</v>
       </c>
@@ -6513,32 +6513,32 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="264"/>
       <c r="G10" s="46"/>
       <c r="I10" s="45">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J10" s="274"/>
+      <c r="J10" s="264"/>
       <c r="K10" s="46"/>
-      <c r="M10" s="264"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M10" s="268"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D11" s="21"/>
       <c r="E11" s="10"/>
       <c r="F11" s="21"/>
       <c r="I11" s="10"/>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D12" s="21"/>
       <c r="E12" s="10"/>
       <c r="F12" s="21"/>
       <c r="I12" s="10"/>
       <c r="J12" s="21"/>
     </row>
-    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="267" t="s">
+    <row r="13" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="265" t="s">
         <v>177</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -6549,7 +6549,7 @@
         <f>'P&amp;L'!D28</f>
         <v>19826.000000000004</v>
       </c>
-      <c r="F13" s="273" t="s">
+      <c r="F13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="72">
@@ -6560,19 +6560,19 @@
         <f>'P&amp;L'!E28</f>
         <v>15605.000000000004</v>
       </c>
-      <c r="J13" s="273" t="s">
+      <c r="J13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K13" s="72">
         <f>I13/I14</f>
         <v>8.6626586951332588E-2</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="267" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="268"/>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B14" s="266"/>
       <c r="C14" s="41" t="s">
         <v>54</v>
       </c>
@@ -6581,18 +6581,18 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="264"/>
       <c r="G14" s="46"/>
       <c r="I14" s="45">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="264"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="264"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B17" s="267" t="s">
+      <c r="M14" s="268"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B17" s="265" t="s">
         <v>178</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -6603,7 +6603,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F17" s="273" t="s">
+      <c r="F17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="72">
@@ -6614,19 +6614,19 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J17" s="273" t="s">
+      <c r="J17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="72">
         <f>I17/I18</f>
         <v>7.7505953669625482E-2</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="267" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="268"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B18" s="266"/>
       <c r="C18" s="41" t="s">
         <v>54</v>
       </c>
@@ -6635,18 +6635,18 @@
         <f>'P&amp;L'!D13</f>
         <v>198845</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="264"/>
       <c r="G18" s="46"/>
       <c r="I18" s="45">
         <f>'P&amp;L'!E13</f>
         <v>180141</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="264"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="264"/>
-    </row>
-    <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="267" t="s">
+      <c r="M18" s="268"/>
+    </row>
+    <row r="21" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="265" t="s">
         <v>149</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -6657,7 +6657,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F21" s="273" t="s">
+      <c r="F21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="72">
@@ -6668,19 +6668,19 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J21" s="273" t="s">
+      <c r="J21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K21" s="72">
         <f>I21/I22</f>
         <v>8.4663592290410331E-2</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="267" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="268"/>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B22" s="266"/>
       <c r="C22" s="41" t="s">
         <v>55</v>
       </c>
@@ -6689,17 +6689,17 @@
         <f>AVERAGE(BS!D23:E23)</f>
         <v>174755.5</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="264"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>AVERAGE(BS!E23:F23)</f>
         <v>164911.5</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="264"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="264"/>
-    </row>
-    <row r="23" spans="2:13" ht="12" x14ac:dyDescent="0.2">
+      <c r="M22" s="268"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B23" s="61"/>
       <c r="C23" s="56"/>
       <c r="D23" s="21"/>
@@ -6711,8 +6711,8 @@
       <c r="K23" s="35"/>
       <c r="M23" s="17"/>
     </row>
-    <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="267" t="s">
+    <row r="25" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="265" t="s">
         <v>150</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -6723,7 +6723,7 @@
         <f>'P&amp;L'!D24</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F25" s="273" t="s">
+      <c r="F25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G25" s="72">
@@ -6734,19 +6734,19 @@
         <f>'P&amp;L'!E24</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J25" s="273" t="s">
+      <c r="J25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K25" s="72">
         <f>I25/I26</f>
         <v>0.11276957640916493</v>
       </c>
-      <c r="M25" s="263" t="s">
+      <c r="M25" s="267" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="268"/>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B26" s="266"/>
       <c r="C26" s="41" t="s">
         <v>55</v>
       </c>
@@ -6755,18 +6755,18 @@
         <f>E22</f>
         <v>174755.5</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="264"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>I22</f>
         <v>164911.5</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="264"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="264"/>
-    </row>
-    <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="267" t="s">
+      <c r="M26" s="268"/>
+    </row>
+    <row r="29" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="265" t="s">
         <v>158</v>
       </c>
       <c r="C29" s="40" t="s">
@@ -6777,7 +6777,7 @@
         <f>E25</f>
         <v>22551.000000000004</v>
       </c>
-      <c r="F29" s="273" t="s">
+      <c r="F29" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G29" s="72">
@@ -6788,19 +6788,19 @@
         <f>I25</f>
         <v>18597.000000000004</v>
       </c>
-      <c r="J29" s="273" t="s">
+      <c r="J29" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K29" s="72">
         <f>I29/I30</f>
         <v>0.1276687765161397</v>
       </c>
-      <c r="M29" s="263" t="s">
+      <c r="M29" s="267" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="268"/>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B30" s="266"/>
       <c r="C30" s="41" t="s">
         <v>86</v>
       </c>
@@ -6809,18 +6809,18 @@
         <f>AVERAGE(BS!D32:E32)+AVERAGE(BS!D36:E36)+AVERAGE(BS!D42:E42)</f>
         <v>154855</v>
       </c>
-      <c r="F30" s="274"/>
+      <c r="F30" s="264"/>
       <c r="G30" s="46"/>
       <c r="I30" s="45">
         <f>AVERAGE(BS!E32:F32)+AVERAGE(BS!E36:F36)+AVERAGE(BS!E42:F42)</f>
         <v>145666</v>
       </c>
-      <c r="J30" s="274"/>
+      <c r="J30" s="264"/>
       <c r="K30" s="46"/>
-      <c r="M30" s="264"/>
-    </row>
-    <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="275" t="s">
+      <c r="M30" s="268"/>
+    </row>
+    <row r="33" spans="2:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="277" t="s">
         <v>168</v>
       </c>
       <c r="C33" s="247" t="s">
@@ -6831,7 +6831,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F33" s="277" t="s">
+      <c r="F33" s="275" t="s">
         <v>44</v>
       </c>
       <c r="G33" s="249">
@@ -6843,19 +6843,19 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J33" s="277" t="s">
+      <c r="J33" s="275" t="s">
         <v>44</v>
       </c>
       <c r="K33" s="249">
         <f>I33/I34</f>
         <v>0.13136687601439562</v>
       </c>
-      <c r="M33" s="263" t="s">
+      <c r="M33" s="267" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="276"/>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.15">
+      <c r="B34" s="278"/>
       <c r="C34" s="250" t="s">
         <v>96</v>
       </c>
@@ -6864,22 +6864,45 @@
         <f>AVERAGE(BS!D32:E32)</f>
         <v>122610</v>
       </c>
-      <c r="F34" s="278"/>
+      <c r="F34" s="276"/>
       <c r="G34" s="201"/>
       <c r="H34" s="73"/>
       <c r="I34" s="251">
         <f>AVERAGE(BS!E32:F32)</f>
         <v>106282.5</v>
       </c>
-      <c r="J34" s="278"/>
+      <c r="J34" s="276"/>
       <c r="K34" s="201"/>
-      <c r="M34" s="264"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M34" s="268"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.15">
       <c r="D35" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F21:F22"/>
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F9:F10"/>
@@ -6892,29 +6915,6 @@
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="M29:M30"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M21:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6930,25 +6930,25 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="3"/>
+    <col min="12" max="12" width="2.83203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="37.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B3" s="269" t="s">
         <v>105</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.15">
       <c r="D4" s="21"/>
       <c r="E4" s="10"/>
       <c r="F4" s="21"/>
@@ -6978,8 +6978,8 @@
       <c r="J4" s="21"/>
       <c r="M4" s="76"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="267" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B5" s="265" t="s">
         <v>181</v>
       </c>
       <c r="C5" s="40" t="s">
@@ -6990,7 +6990,7 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F5" s="273" t="s">
+      <c r="F5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="71">
@@ -7001,19 +7001,19 @@
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J5" s="273" t="s">
+      <c r="J5" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K5" s="113">
         <f>I5/I6</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="M5" s="263" t="s">
+      <c r="M5" s="267" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="268"/>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B6" s="266"/>
       <c r="C6" s="41" t="s">
         <v>183</v>
       </c>
@@ -7022,17 +7022,17 @@
         <f>'P&amp;L'!D50</f>
         <v>10000</v>
       </c>
-      <c r="F6" s="274"/>
+      <c r="F6" s="264"/>
       <c r="G6" s="46"/>
       <c r="I6" s="65">
         <f>'P&amp;L'!E50</f>
         <v>10000</v>
       </c>
-      <c r="J6" s="274"/>
+      <c r="J6" s="264"/>
       <c r="K6" s="46"/>
-      <c r="M6" s="264"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M6" s="268"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I7" s="73"/>
       <c r="J7" s="73"/>
       <c r="K7" s="73"/>
@@ -7041,7 +7041,7 @@
       <c r="N7" s="73"/>
       <c r="O7" s="73"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I8" s="73"/>
       <c r="J8" s="73"/>
       <c r="K8" s="73"/>
@@ -7050,8 +7050,8 @@
       <c r="N8" s="73"/>
       <c r="O8" s="73"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="267" t="s">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B9" s="265" t="s">
         <v>187</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -7061,7 +7061,7 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F9" s="273" t="s">
+      <c r="F9" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G9" s="71">
@@ -7072,7 +7072,7 @@
         <f>'P&amp;L'!E53</f>
         <v>2.15</v>
       </c>
-      <c r="J9" s="277" t="s">
+      <c r="J9" s="275" t="s">
         <v>44</v>
       </c>
       <c r="K9" s="199">
@@ -7080,14 +7080,14 @@
         <v>1.5398939979945563</v>
       </c>
       <c r="L9" s="73"/>
-      <c r="M9" s="279" t="s">
+      <c r="M9" s="281" t="s">
         <v>191</v>
       </c>
       <c r="N9" s="73"/>
       <c r="O9" s="73"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="268"/>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B10" s="266"/>
       <c r="C10" s="41" t="s">
         <v>189</v>
       </c>
@@ -7095,20 +7095,20 @@
         <f>G5</f>
         <v>1.7698000000000003</v>
       </c>
-      <c r="F10" s="274"/>
+      <c r="F10" s="264"/>
       <c r="G10" s="46"/>
       <c r="I10" s="200">
         <f>K5</f>
         <v>1.3962000000000003</v>
       </c>
-      <c r="J10" s="278"/>
+      <c r="J10" s="276"/>
       <c r="K10" s="201"/>
       <c r="L10" s="73"/>
-      <c r="M10" s="280"/>
+      <c r="M10" s="282"/>
       <c r="N10" s="73"/>
       <c r="O10" s="73"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I11" s="73"/>
       <c r="J11" s="73"/>
       <c r="K11" s="73"/>
@@ -7117,8 +7117,8 @@
       <c r="N11" s="73"/>
       <c r="O11" s="73"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="267" t="s">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B13" s="265" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -7128,7 +7128,7 @@
         <f>'P&amp;L'!D54</f>
         <v>29500</v>
       </c>
-      <c r="F13" s="273" t="s">
+      <c r="F13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="71">
@@ -7139,19 +7139,19 @@
         <f>'P&amp;L'!E54</f>
         <v>21500</v>
       </c>
-      <c r="J13" s="273" t="s">
+      <c r="J13" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K13" s="113">
         <f>I13/I14</f>
         <v>1.5398939979945563</v>
       </c>
-      <c r="M13" s="263" t="s">
+      <c r="M13" s="267" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="268"/>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B14" s="266"/>
       <c r="C14" s="41" t="s">
         <v>97</v>
       </c>
@@ -7159,18 +7159,18 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F14" s="274"/>
+      <c r="F14" s="264"/>
       <c r="G14" s="46"/>
       <c r="I14" s="120">
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J14" s="274"/>
+      <c r="J14" s="264"/>
       <c r="K14" s="46"/>
-      <c r="M14" s="264"/>
-    </row>
-    <row r="17" spans="2:15" ht="12" x14ac:dyDescent="0.25">
-      <c r="B17" s="267" t="s">
+      <c r="M14" s="268"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B17" s="265" t="s">
         <v>195</v>
       </c>
       <c r="C17" s="40" t="s">
@@ -7180,7 +7180,7 @@
         <f>'P&amp;L'!D51</f>
         <v>0.88</v>
       </c>
-      <c r="F17" s="273" t="s">
+      <c r="F17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="252">
@@ -7191,19 +7191,19 @@
         <f>'P&amp;L'!E51</f>
         <v>0.65</v>
       </c>
-      <c r="J17" s="273" t="s">
+      <c r="J17" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K17" s="252">
         <f>I17/I18</f>
         <v>0.30232558139534887</v>
       </c>
-      <c r="M17" s="263" t="s">
+      <c r="M17" s="267" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="268"/>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B18" s="266"/>
       <c r="C18" s="41" t="s">
         <v>196</v>
       </c>
@@ -7211,18 +7211,18 @@
         <f>'P&amp;L'!D53</f>
         <v>2.95</v>
       </c>
-      <c r="F18" s="274"/>
+      <c r="F18" s="264"/>
       <c r="G18" s="46"/>
       <c r="I18" s="117">
         <f>'P&amp;L'!E53</f>
         <v>2.15</v>
       </c>
-      <c r="J18" s="274"/>
+      <c r="J18" s="264"/>
       <c r="K18" s="46"/>
-      <c r="M18" s="264"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="267" t="s">
+      <c r="M18" s="268"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B21" s="265" t="s">
         <v>199</v>
       </c>
       <c r="C21" s="40" t="s">
@@ -7232,7 +7232,7 @@
         <f>'P&amp;L'!D32-'P&amp;L'!D52</f>
         <v>8898.0000000000036</v>
       </c>
-      <c r="F21" s="273" t="s">
+      <c r="F21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G21" s="66">
@@ -7243,20 +7243,20 @@
         <f>'P&amp;L'!E32-'P&amp;L'!E52</f>
         <v>7462.0000000000036</v>
       </c>
-      <c r="J21" s="273" t="s">
+      <c r="J21" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K21" s="66">
         <f>I21/I22</f>
         <v>0.53445065176908768</v>
       </c>
-      <c r="M21" s="263" t="s">
+      <c r="M21" s="267" t="s">
         <v>204</v>
       </c>
       <c r="O21" s="130"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="268"/>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B22" s="266"/>
       <c r="C22" s="41" t="s">
         <v>202</v>
       </c>
@@ -7264,18 +7264,18 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F22" s="274"/>
+      <c r="F22" s="264"/>
       <c r="G22" s="46"/>
       <c r="I22" s="45">
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J22" s="274"/>
+      <c r="J22" s="264"/>
       <c r="K22" s="46"/>
-      <c r="M22" s="264"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B25" s="267" t="s">
+      <c r="M22" s="268"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B25" s="265" t="s">
         <v>205</v>
       </c>
       <c r="C25" s="40" t="s">
@@ -7285,7 +7285,7 @@
         <f>'P&amp;L'!D52</f>
         <v>8800</v>
       </c>
-      <c r="F25" s="273" t="s">
+      <c r="F25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="G25" s="66">
@@ -7296,19 +7296,19 @@
         <f>'P&amp;L'!E52</f>
         <v>6500</v>
       </c>
-      <c r="J25" s="273" t="s">
+      <c r="J25" s="263" t="s">
         <v>44</v>
       </c>
       <c r="K25" s="66">
         <f>I25/I26</f>
         <v>0.46554934823091237</v>
       </c>
-      <c r="M25" s="263" t="s">
+      <c r="M25" s="267" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B26" s="268"/>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B26" s="266"/>
       <c r="C26" s="41" t="s">
         <v>202</v>
       </c>
@@ -7316,21 +7316,21 @@
         <f>'P&amp;L'!D32</f>
         <v>17698.000000000004</v>
       </c>
-      <c r="F26" s="274"/>
+      <c r="F26" s="264"/>
       <c r="G26" s="46"/>
       <c r="I26" s="45">
         <f>'P&amp;L'!E32</f>
         <v>13962.000000000004</v>
       </c>
-      <c r="J26" s="274"/>
+      <c r="J26" s="264"/>
       <c r="K26" s="46"/>
-      <c r="M26" s="264"/>
-    </row>
-    <row r="29" spans="2:15" ht="12" x14ac:dyDescent="0.25">
-      <c r="B29" s="281" t="s">
+      <c r="M26" s="268"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B29" s="279" t="s">
         <v>208</v>
       </c>
-      <c r="C29" s="282"/>
+      <c r="C29" s="280"/>
       <c r="E29" s="133"/>
       <c r="F29" s="134"/>
       <c r="G29" s="135">
@@ -7349,15 +7349,12 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="J17:J18"/>
@@ -7371,12 +7368,15 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="M13:M14"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="M25:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7390,28 +7390,30 @@
   </sheetPr>
   <dimension ref="B1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="163" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="163" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="163" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="13.1640625" style="163" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="163" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="163" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="D2" s="286" t="s">
         <v>143</v>
       </c>
       <c r="E2" s="287"/>
     </row>
-    <row r="3" spans="2:7" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="162" t="s">
         <v>221</v>
       </c>
@@ -7431,12 +7433,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
       <c r="E4" s="165"/>
       <c r="F4" s="165"/>
       <c r="G4" s="165"/>
     </row>
-    <row r="5" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B5" s="288" t="s">
         <v>258</v>
       </c>
@@ -7458,7 +7460,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B6" s="289"/>
       <c r="C6" s="167" t="s">
         <v>255</v>
@@ -7479,7 +7481,7 @@
         <v>50.3</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B7" s="289"/>
       <c r="C7" s="167" t="s">
         <v>256</v>
@@ -7499,7 +7501,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B8" s="289"/>
       <c r="C8" s="167" t="s">
         <v>257</v>
@@ -7521,7 +7523,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B9" s="290"/>
       <c r="C9" s="168" t="s">
         <v>90</v>
@@ -7541,11 +7543,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
       <c r="D10" s="163"/>
       <c r="G10" s="165"/>
     </row>
-    <row r="11" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B11" s="283" t="s">
         <v>260</v>
       </c>
@@ -7567,7 +7569,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B12" s="284"/>
       <c r="C12" s="35" t="s">
         <v>259</v>
@@ -7587,7 +7589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B13" s="285"/>
       <c r="C13" s="58" t="s">
         <v>268</v>
@@ -7607,11 +7609,11 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
       <c r="D14" s="163"/>
       <c r="G14" s="165"/>
     </row>
-    <row r="15" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B15" s="283" t="s">
         <v>270</v>
       </c>
@@ -7633,7 +7635,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B16" s="284"/>
       <c r="C16" s="35" t="s">
         <v>267</v>
@@ -7653,7 +7655,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="285"/>
       <c r="C17" s="58" t="s">
         <v>269</v>
@@ -7673,12 +7675,12 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="159"/>
       <c r="D18" s="163"/>
       <c r="G18" s="165"/>
     </row>
-    <row r="19" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B19" s="283" t="s">
         <v>261</v>
       </c>
@@ -7700,7 +7702,7 @@
         <v>0.29499999999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B20" s="284"/>
       <c r="C20" s="35" t="s">
         <v>271</v>
@@ -7720,7 +7722,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="284"/>
       <c r="C21" s="35" t="s">
         <v>91</v>
@@ -7740,7 +7742,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="285"/>
       <c r="C22" s="58" t="s">
         <v>169</v>
@@ -7762,11 +7764,11 @@
       <c r="H22" s="146"/>
       <c r="I22" s="146"/>
     </row>
-    <row r="23" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
       <c r="D23" s="163"/>
       <c r="G23" s="165"/>
     </row>
-    <row r="24" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="283" t="s">
         <v>263</v>
       </c>
@@ -7788,7 +7790,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B25" s="284"/>
       <c r="C25" s="35" t="s">
         <v>265</v>
@@ -7808,7 +7810,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B26" s="285"/>
       <c r="C26" s="58" t="s">
         <v>188</v>
@@ -7860,19 +7862,19 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="3"/>
-    <col min="4" max="4" width="9.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="2.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="3"/>
+    <col min="4" max="4" width="9.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="3"/>
     <col min="6" max="6" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="8.5" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="39" x14ac:dyDescent="0.15">
       <c r="B2" s="155" t="s">
         <v>276</v>
       </c>
@@ -7886,7 +7888,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
         <v>87</v>
       </c>
@@ -7916,7 +7918,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B4" s="6"/>
       <c r="C4" s="2"/>
       <c r="E4" s="5"/>
@@ -7927,7 +7929,7 @@
       <c r="J4" s="147"/>
       <c r="K4" s="147"/>
     </row>
-    <row r="5" spans="2:11" ht="12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
@@ -7964,7 +7966,7 @@
         <v>304852.46269865491</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B6" s="142" t="s">
         <v>232</v>
       </c>
@@ -7984,7 +7986,7 @@
       <c r="J6" s="154"/>
       <c r="K6" s="154"/>
     </row>
-    <row r="7" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B7" s="144" t="s">
         <v>236</v>
       </c>
@@ -8020,7 +8022,7 @@
         <v>-225189.48278453248</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B8" s="142" t="s">
         <v>232</v>
       </c>
@@ -8055,7 +8057,7 @@
         <v>8.4232797636980106E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B9" s="144" t="s">
         <v>39</v>
       </c>
@@ -8092,7 +8094,7 @@
         <v>79662.979914122436</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B10" s="142" t="s">
         <v>232</v>
       </c>
@@ -8112,7 +8114,7 @@
       <c r="J10" s="154"/>
       <c r="K10" s="154"/>
     </row>
-    <row r="11" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B11" s="144" t="s">
         <v>226</v>
       </c>
@@ -8149,7 +8151,7 @@
         <v>0.26131650441305077</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B12" s="142" t="s">
         <v>237</v>
       </c>
@@ -8182,21 +8184,21 @@
         <v>1.3661152479096689E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.15">
       <c r="G13" s="73"/>
       <c r="H13" s="73"/>
       <c r="I13" s="73"/>
       <c r="J13" s="73"/>
       <c r="K13" s="73"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.15">
       <c r="G14" s="73"/>
       <c r="H14" s="73"/>
       <c r="I14" s="73"/>
       <c r="J14" s="73"/>
       <c r="K14" s="73"/>
     </row>
-    <row r="15" spans="2:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="39" x14ac:dyDescent="0.15">
       <c r="B15" s="156" t="s">
         <v>240</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>87</v>
       </c>
@@ -8240,7 +8242,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B17" s="6"/>
       <c r="C17" s="2"/>
       <c r="E17" s="5"/>
@@ -8251,7 +8253,7 @@
       <c r="J17" s="147"/>
       <c r="K17" s="147"/>
     </row>
-    <row r="18" spans="2:11" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
@@ -8289,7 +8291,7 @@
         <v>297939.0145485634</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B19" s="142" t="s">
         <v>232</v>
       </c>
@@ -8309,7 +8311,7 @@
       <c r="J19" s="154"/>
       <c r="K19" s="154"/>
     </row>
-    <row r="20" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B20" s="144" t="s">
         <v>236</v>
       </c>
@@ -8346,7 +8348,7 @@
         <v>-225189.48278453248</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B21" s="142" t="s">
         <v>232</v>
       </c>
@@ -8381,7 +8383,7 @@
         <v>8.4232797636980106E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B22" s="144" t="s">
         <v>39</v>
       </c>
@@ -8418,7 +8420,7 @@
         <v>72749.531764030922</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B23" s="142" t="s">
         <v>232</v>
       </c>
@@ -8438,7 +8440,7 @@
       <c r="J23" s="154"/>
       <c r="K23" s="154"/>
     </row>
-    <row r="24" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B24" s="144" t="s">
         <v>226</v>
       </c>
@@ -8475,7 +8477,7 @@
         <v>0.24417591591440571</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B25" s="142" t="s">
         <v>237</v>
       </c>
@@ -8507,7 +8509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="39" x14ac:dyDescent="0.15">
       <c r="B28" s="157" t="s">
         <v>241</v>
       </c>
@@ -8521,7 +8523,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B29" s="23" t="s">
         <v>87</v>
       </c>
@@ -8551,7 +8553,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B30" s="6"/>
       <c r="C30" s="2"/>
       <c r="E30" s="5"/>
@@ -8562,7 +8564,7 @@
       <c r="J30" s="147"/>
       <c r="K30" s="147"/>
     </row>
-    <row r="31" spans="2:11" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" ht="13" x14ac:dyDescent="0.15">
       <c r="B31" s="6" t="s">
         <v>26</v>
       </c>
@@ -8600,7 +8602,7 @@
         <v>327137.79588296841</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B32" s="142" t="s">
         <v>232</v>
       </c>
@@ -8620,7 +8622,7 @@
       <c r="J32" s="154"/>
       <c r="K32" s="154"/>
     </row>
-    <row r="33" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B33" s="144" t="s">
         <v>236</v>
       </c>
@@ -8657,7 +8659,7 @@
         <v>-225189.48278453248</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B34" s="142" t="s">
         <v>232</v>
       </c>
@@ -8692,7 +8694,7 @@
         <v>8.4232797636980106E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B35" s="144" t="s">
         <v>39</v>
       </c>
@@ -8729,7 +8731,7 @@
         <v>101948.31309843593</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B36" s="142" t="s">
         <v>232</v>
       </c>
@@ -8749,7 +8751,7 @@
       <c r="J36" s="154"/>
       <c r="K36" s="154"/>
     </row>
-    <row r="37" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B37" s="144" t="s">
         <v>226</v>
       </c>
@@ -8786,7 +8788,7 @@
         <v>0.31163721948810635</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B38" s="142" t="s">
         <v>237</v>
       </c>

</xml_diff>